<commit_message>
Revisado relatorio de backtracking
</commit_message>
<xml_diff>
--- a/analises/analise-backtracking.xlsx
+++ b/analises/analise-backtracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Documentos\02 - Repositorios\02 - Repositorios faculdade\leilaodeenergia-tp-grupo-alunossemgrupo\analises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6017B8FC-42EC-4B36-B60B-CC6CA2994635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976B87E7-9806-4DD8-B939-7FEBE2514AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{12248BD6-8FAC-4B11-9F3D-44074F5654BF}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8874" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8879" uniqueCount="245">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -766,6 +766,18 @@
   <si>
     <t>Melhor lucro médio</t>
   </si>
+  <si>
+    <t>Conjunto</t>
+  </si>
+  <si>
+    <t>Um</t>
+  </si>
+  <si>
+    <t>Dois</t>
+  </si>
+  <si>
+    <t>Lances selecionados</t>
+  </si>
 </sst>
 </file>
 
@@ -773,7 +785,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -935,14 +947,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2852,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709D3D01-8D35-45FA-AB2C-61E9B06F1F4F}">
   <dimension ref="A1:L281"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G16"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10795,8 +10807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD8B2C1-76F9-4A22-BD1B-85D28A0AA152}">
   <dimension ref="B3:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10805,20 +10817,24 @@
     <col min="2" max="2" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="11.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:20" ht="15" customHeight="1">
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:20" ht="30">
       <c r="B4" s="21" t="s">
@@ -10857,6 +10873,15 @@
       <c r="M4" s="21" t="s">
         <v>237</v>
       </c>
+      <c r="P4" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q4" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="5" spans="2:20">
       <c r="B5" s="18">
@@ -10906,6 +10931,12 @@
         <f>AVERAGE(C5:L5)</f>
         <v>0</v>
       </c>
+      <c r="P5" s="18">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="18">
@@ -10955,6 +10986,12 @@
         <f t="shared" ref="M6:M32" si="0">AVERAGE(C6:L6)</f>
         <v>0</v>
       </c>
+      <c r="P6" s="18">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="7" spans="2:20">
       <c r="B7" s="18">
@@ -12232,7 +12269,7 @@
       </c>
       <c r="W32" s="22"/>
     </row>
-    <row r="34" spans="2:13" ht="45">
+    <row r="34" spans="2:16" ht="45">
       <c r="B34" s="21" t="s">
         <v>239</v>
       </c>
@@ -12269,689 +12306,690 @@
       <c r="M34" s="21" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="35" spans="2:13">
+      <c r="P34" s="21"/>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="18">
         <v>10</v>
       </c>
-      <c r="C35" s="24">
+      <c r="C35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!C$4)</f>
         <v>504</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!D$4)</f>
         <v>393</v>
       </c>
-      <c r="E35" s="24">
+      <c r="E35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!E$4)</f>
         <v>408</v>
       </c>
-      <c r="F35" s="24">
+      <c r="F35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!F$4)</f>
         <v>580</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!G$4)</f>
         <v>248</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!H$4)</f>
         <v>341</v>
       </c>
-      <c r="I35" s="24">
+      <c r="I35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!I$4)</f>
         <v>372</v>
       </c>
-      <c r="J35" s="24">
+      <c r="J35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!J$4)</f>
         <v>449</v>
       </c>
-      <c r="K35" s="24">
+      <c r="K35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!K$4)</f>
         <v>531</v>
       </c>
-      <c r="L35" s="24">
+      <c r="L35" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B35,exec!$L:$L,tabela!L$4)</f>
         <v>467</v>
       </c>
-      <c r="M35" s="25">
+      <c r="M35" s="24">
         <f>AVERAGE(C35:L35)</f>
         <v>429.3</v>
       </c>
     </row>
-    <row r="36" spans="2:13">
+    <row r="36" spans="2:16">
       <c r="B36" s="18">
         <v>11</v>
       </c>
-      <c r="C36" s="24">
+      <c r="C36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!C$4)</f>
         <v>361</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!D$4)</f>
         <v>388</v>
       </c>
-      <c r="E36" s="24">
+      <c r="E36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!E$4)</f>
         <v>548</v>
       </c>
-      <c r="F36" s="24">
+      <c r="F36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!F$4)</f>
         <v>613</v>
       </c>
-      <c r="G36" s="24">
+      <c r="G36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!G$4)</f>
         <v>561</v>
       </c>
-      <c r="H36" s="24">
+      <c r="H36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!H$4)</f>
         <v>627</v>
       </c>
-      <c r="I36" s="24">
+      <c r="I36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!I$4)</f>
         <v>424</v>
       </c>
-      <c r="J36" s="24">
+      <c r="J36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!J$4)</f>
         <v>648</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!K$4)</f>
         <v>597</v>
       </c>
-      <c r="L36" s="24">
+      <c r="L36" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B36,exec!$L:$L,tabela!L$4)</f>
         <v>442</v>
       </c>
-      <c r="M36" s="25">
+      <c r="M36" s="24">
         <f t="shared" ref="M36:M62" si="1">AVERAGE(C36:L36)</f>
         <v>520.9</v>
       </c>
     </row>
-    <row r="37" spans="2:13">
+    <row r="37" spans="2:16">
       <c r="B37" s="18">
         <v>12</v>
       </c>
-      <c r="C37" s="24">
+      <c r="C37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!C$4)</f>
         <v>574</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!D$4)</f>
         <v>459</v>
       </c>
-      <c r="E37" s="24">
+      <c r="E37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!E$4)</f>
         <v>618</v>
       </c>
-      <c r="F37" s="24">
+      <c r="F37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!F$4)</f>
         <v>465</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!G$4)</f>
         <v>511</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!H$4)</f>
         <v>368</v>
       </c>
-      <c r="I37" s="24">
+      <c r="I37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!I$4)</f>
         <v>334</v>
       </c>
-      <c r="J37" s="24">
+      <c r="J37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!J$4)</f>
         <v>376</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!K$4)</f>
         <v>650</v>
       </c>
-      <c r="L37" s="24">
+      <c r="L37" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B37,exec!$L:$L,tabela!L$4)</f>
         <v>651</v>
       </c>
-      <c r="M37" s="25">
+      <c r="M37" s="24">
         <f t="shared" si="1"/>
         <v>500.6</v>
       </c>
     </row>
-    <row r="38" spans="2:13">
+    <row r="38" spans="2:16">
       <c r="B38" s="18">
         <v>13</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!C$4)</f>
         <v>514</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!D$4)</f>
         <v>653</v>
       </c>
-      <c r="E38" s="24">
+      <c r="E38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!E$4)</f>
         <v>428</v>
       </c>
-      <c r="F38" s="24">
+      <c r="F38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!F$4)</f>
         <v>459</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!G$4)</f>
         <v>672</v>
       </c>
-      <c r="H38" s="24">
+      <c r="H38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!H$4)</f>
         <v>602</v>
       </c>
-      <c r="I38" s="24">
+      <c r="I38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!I$4)</f>
         <v>610</v>
       </c>
-      <c r="J38" s="24">
+      <c r="J38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!J$4)</f>
         <v>537</v>
       </c>
-      <c r="K38" s="24">
+      <c r="K38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!K$4)</f>
         <v>555</v>
       </c>
-      <c r="L38" s="24">
+      <c r="L38" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B38,exec!$L:$L,tabela!L$4)</f>
         <v>626</v>
       </c>
-      <c r="M38" s="25">
+      <c r="M38" s="24">
         <f t="shared" si="1"/>
         <v>565.6</v>
       </c>
     </row>
-    <row r="39" spans="2:13">
+    <row r="39" spans="2:16">
       <c r="B39" s="18">
         <v>14</v>
       </c>
-      <c r="C39" s="24">
+      <c r="C39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!C$4)</f>
         <v>573</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!D$4)</f>
         <v>687</v>
       </c>
-      <c r="E39" s="24">
+      <c r="E39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!E$4)</f>
         <v>822</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!F$4)</f>
         <v>641</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!G$4)</f>
         <v>454</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!H$4)</f>
         <v>555</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!I$4)</f>
         <v>673</v>
       </c>
-      <c r="J39" s="24">
+      <c r="J39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!J$4)</f>
         <v>420</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!K$4)</f>
         <v>551</v>
       </c>
-      <c r="L39" s="24">
+      <c r="L39" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B39,exec!$L:$L,tabela!L$4)</f>
         <v>528</v>
       </c>
-      <c r="M39" s="25">
+      <c r="M39" s="24">
         <f t="shared" si="1"/>
         <v>590.4</v>
       </c>
     </row>
-    <row r="40" spans="2:13">
+    <row r="40" spans="2:16">
       <c r="B40" s="18">
         <v>15</v>
       </c>
-      <c r="C40" s="24">
+      <c r="C40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!C$4)</f>
         <v>765</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!D$4)</f>
         <v>536</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!E$4)</f>
         <v>499</v>
       </c>
-      <c r="F40" s="24">
+      <c r="F40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!F$4)</f>
         <v>654</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!G$4)</f>
         <v>578</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!H$4)</f>
         <v>465</v>
       </c>
-      <c r="I40" s="24">
+      <c r="I40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!I$4)</f>
         <v>571</v>
       </c>
-      <c r="J40" s="24">
+      <c r="J40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!J$4)</f>
         <v>628</v>
       </c>
-      <c r="K40" s="24">
+      <c r="K40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!K$4)</f>
         <v>577</v>
       </c>
-      <c r="L40" s="24">
+      <c r="L40" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B40,exec!$L:$L,tabela!L$4)</f>
         <v>563</v>
       </c>
-      <c r="M40" s="25">
+      <c r="M40" s="24">
         <f t="shared" si="1"/>
         <v>583.6</v>
       </c>
     </row>
-    <row r="41" spans="2:13">
+    <row r="41" spans="2:16">
       <c r="B41" s="18">
         <v>16</v>
       </c>
-      <c r="C41" s="24">
+      <c r="C41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!C$4)</f>
         <v>697</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!D$4)</f>
         <v>777</v>
       </c>
-      <c r="E41" s="24">
+      <c r="E41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!E$4)</f>
         <v>573</v>
       </c>
-      <c r="F41" s="24">
+      <c r="F41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!F$4)</f>
         <v>614</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!G$4)</f>
         <v>569</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!H$4)</f>
         <v>671</v>
       </c>
-      <c r="I41" s="24">
+      <c r="I41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!I$4)</f>
         <v>618</v>
       </c>
-      <c r="J41" s="24">
+      <c r="J41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!J$4)</f>
         <v>696</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!K$4)</f>
         <v>794</v>
       </c>
-      <c r="L41" s="24">
+      <c r="L41" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B41,exec!$L:$L,tabela!L$4)</f>
         <v>659</v>
       </c>
-      <c r="M41" s="25">
+      <c r="M41" s="24">
         <f t="shared" si="1"/>
         <v>666.8</v>
       </c>
     </row>
-    <row r="42" spans="2:13">
+    <row r="42" spans="2:16">
       <c r="B42" s="18">
         <v>17</v>
       </c>
-      <c r="C42" s="24">
+      <c r="C42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!C$4)</f>
         <v>792</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!D$4)</f>
         <v>813</v>
       </c>
-      <c r="E42" s="24">
+      <c r="E42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!E$4)</f>
         <v>658</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!F$4)</f>
         <v>646</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!G$4)</f>
         <v>812</v>
       </c>
-      <c r="H42" s="24">
+      <c r="H42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!H$4)</f>
         <v>501</v>
       </c>
-      <c r="I42" s="24">
+      <c r="I42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!I$4)</f>
         <v>769</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!J$4)</f>
         <v>755</v>
       </c>
-      <c r="K42" s="24">
+      <c r="K42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!K$4)</f>
         <v>625</v>
       </c>
-      <c r="L42" s="24">
+      <c r="L42" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B42,exec!$L:$L,tabela!L$4)</f>
         <v>795</v>
       </c>
-      <c r="M42" s="25">
+      <c r="M42" s="24">
         <f t="shared" si="1"/>
         <v>716.6</v>
       </c>
     </row>
-    <row r="43" spans="2:13">
+    <row r="43" spans="2:16">
       <c r="B43" s="18">
         <v>18</v>
       </c>
-      <c r="C43" s="24">
+      <c r="C43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!C$4)</f>
         <v>568</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!D$4)</f>
         <v>607</v>
       </c>
-      <c r="E43" s="24">
+      <c r="E43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!E$4)</f>
         <v>827</v>
       </c>
-      <c r="F43" s="24">
+      <c r="F43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!F$4)</f>
         <v>511</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!G$4)</f>
         <v>589</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!H$4)</f>
         <v>810</v>
       </c>
-      <c r="I43" s="24">
+      <c r="I43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!I$4)</f>
         <v>724</v>
       </c>
-      <c r="J43" s="24">
+      <c r="J43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!J$4)</f>
         <v>451</v>
       </c>
-      <c r="K43" s="24">
+      <c r="K43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!K$4)</f>
         <v>714</v>
       </c>
-      <c r="L43" s="24">
+      <c r="L43" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B43,exec!$L:$L,tabela!L$4)</f>
         <v>522</v>
       </c>
-      <c r="M43" s="25">
+      <c r="M43" s="24">
         <f t="shared" si="1"/>
         <v>632.29999999999995</v>
       </c>
     </row>
-    <row r="44" spans="2:13">
+    <row r="44" spans="2:16">
       <c r="B44" s="18">
         <v>19</v>
       </c>
-      <c r="C44" s="24">
+      <c r="C44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!C$4)</f>
         <v>750</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!D$4)</f>
         <v>561</v>
       </c>
-      <c r="E44" s="24">
+      <c r="E44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!E$4)</f>
         <v>829</v>
       </c>
-      <c r="F44" s="24">
+      <c r="F44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!F$4)</f>
         <v>595</v>
       </c>
-      <c r="G44" s="24">
+      <c r="G44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!G$4)</f>
         <v>789</v>
       </c>
-      <c r="H44" s="24">
+      <c r="H44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!H$4)</f>
         <v>544</v>
       </c>
-      <c r="I44" s="24">
+      <c r="I44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!I$4)</f>
         <v>645</v>
       </c>
-      <c r="J44" s="24">
+      <c r="J44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!J$4)</f>
         <v>756</v>
       </c>
-      <c r="K44" s="24">
+      <c r="K44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!K$4)</f>
         <v>864</v>
       </c>
-      <c r="L44" s="24">
+      <c r="L44" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B44,exec!$L:$L,tabela!L$4)</f>
         <v>680</v>
       </c>
-      <c r="M44" s="25">
+      <c r="M44" s="24">
         <f t="shared" si="1"/>
         <v>701.3</v>
       </c>
     </row>
-    <row r="45" spans="2:13">
+    <row r="45" spans="2:16">
       <c r="B45" s="18">
         <v>20</v>
       </c>
-      <c r="C45" s="24">
+      <c r="C45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!C$4)</f>
         <v>612</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!D$4)</f>
         <v>556</v>
       </c>
-      <c r="E45" s="24">
+      <c r="E45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!E$4)</f>
         <v>804</v>
       </c>
-      <c r="F45" s="24">
+      <c r="F45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!F$4)</f>
         <v>707</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!G$4)</f>
         <v>646</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!H$4)</f>
         <v>830</v>
       </c>
-      <c r="I45" s="24">
+      <c r="I45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!I$4)</f>
         <v>1005</v>
       </c>
-      <c r="J45" s="24">
+      <c r="J45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!J$4)</f>
         <v>618</v>
       </c>
-      <c r="K45" s="24">
+      <c r="K45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!K$4)</f>
         <v>690</v>
       </c>
-      <c r="L45" s="24">
+      <c r="L45" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B45,exec!$L:$L,tabela!L$4)</f>
         <v>755</v>
       </c>
-      <c r="M45" s="25">
+      <c r="M45" s="24">
         <f t="shared" si="1"/>
         <v>722.3</v>
       </c>
     </row>
-    <row r="46" spans="2:13">
+    <row r="46" spans="2:16">
       <c r="B46" s="18">
         <v>21</v>
       </c>
-      <c r="C46" s="24">
+      <c r="C46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!C$4)</f>
         <v>663</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!D$4)</f>
         <v>660</v>
       </c>
-      <c r="E46" s="24">
+      <c r="E46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!E$4)</f>
         <v>659</v>
       </c>
-      <c r="F46" s="24">
+      <c r="F46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!F$4)</f>
         <v>871</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!G$4)</f>
         <v>473</v>
       </c>
-      <c r="H46" s="24">
+      <c r="H46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!H$4)</f>
         <v>661</v>
       </c>
-      <c r="I46" s="24">
+      <c r="I46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!I$4)</f>
         <v>734</v>
       </c>
-      <c r="J46" s="24">
+      <c r="J46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!J$4)</f>
         <v>956</v>
       </c>
-      <c r="K46" s="24">
+      <c r="K46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!K$4)</f>
         <v>651</v>
       </c>
-      <c r="L46" s="24">
+      <c r="L46" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B46,exec!$L:$L,tabela!L$4)</f>
         <v>752</v>
       </c>
-      <c r="M46" s="25">
+      <c r="M46" s="24">
         <f t="shared" si="1"/>
         <v>708</v>
       </c>
     </row>
-    <row r="47" spans="2:13">
+    <row r="47" spans="2:16">
       <c r="B47" s="18">
         <v>22</v>
       </c>
-      <c r="C47" s="24">
+      <c r="C47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!C$4)</f>
         <v>599</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!D$4)</f>
         <v>860</v>
       </c>
-      <c r="E47" s="24">
+      <c r="E47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!E$4)</f>
         <v>534</v>
       </c>
-      <c r="F47" s="24">
+      <c r="F47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!F$4)</f>
         <v>817</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!G$4)</f>
         <v>802</v>
       </c>
-      <c r="H47" s="24">
+      <c r="H47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!H$4)</f>
         <v>772</v>
       </c>
-      <c r="I47" s="24">
+      <c r="I47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!I$4)</f>
         <v>769</v>
       </c>
-      <c r="J47" s="24">
+      <c r="J47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!J$4)</f>
         <v>1097</v>
       </c>
-      <c r="K47" s="24">
+      <c r="K47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!K$4)</f>
         <v>832</v>
       </c>
-      <c r="L47" s="24">
+      <c r="L47" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B47,exec!$L:$L,tabela!L$4)</f>
         <v>763</v>
       </c>
-      <c r="M47" s="25">
+      <c r="M47" s="24">
         <f t="shared" si="1"/>
         <v>784.5</v>
       </c>
     </row>
-    <row r="48" spans="2:13">
+    <row r="48" spans="2:16">
       <c r="B48" s="18">
         <v>23</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!C$4)</f>
         <v>549</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!D$4)</f>
         <v>953</v>
       </c>
-      <c r="E48" s="24">
+      <c r="E48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!E$4)</f>
         <v>968</v>
       </c>
-      <c r="F48" s="24">
+      <c r="F48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!F$4)</f>
         <v>813</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!G$4)</f>
         <v>737</v>
       </c>
-      <c r="H48" s="24">
+      <c r="H48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!H$4)</f>
         <v>696</v>
       </c>
-      <c r="I48" s="24">
+      <c r="I48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!I$4)</f>
         <v>878</v>
       </c>
-      <c r="J48" s="24">
+      <c r="J48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!J$4)</f>
         <v>789</v>
       </c>
-      <c r="K48" s="24">
+      <c r="K48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!K$4)</f>
         <v>833</v>
       </c>
-      <c r="L48" s="24">
+      <c r="L48" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B48,exec!$L:$L,tabela!L$4)</f>
         <v>1039</v>
       </c>
-      <c r="M48" s="25">
+      <c r="M48" s="24">
         <f t="shared" si="1"/>
         <v>825.5</v>
       </c>
@@ -12960,47 +12998,47 @@
       <c r="B49" s="18">
         <v>24</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!C$4)</f>
         <v>886</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!D$4)</f>
         <v>855</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!E$4)</f>
         <v>625</v>
       </c>
-      <c r="F49" s="24">
+      <c r="F49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!F$4)</f>
         <v>999</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!G$4)</f>
         <v>663</v>
       </c>
-      <c r="H49" s="24">
+      <c r="H49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!H$4)</f>
         <v>657</v>
       </c>
-      <c r="I49" s="24">
+      <c r="I49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!I$4)</f>
         <v>633</v>
       </c>
-      <c r="J49" s="24">
+      <c r="J49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!J$4)</f>
         <v>877</v>
       </c>
-      <c r="K49" s="24">
+      <c r="K49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!K$4)</f>
         <v>955</v>
       </c>
-      <c r="L49" s="24">
+      <c r="L49" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B49,exec!$L:$L,tabela!L$4)</f>
         <v>886</v>
       </c>
-      <c r="M49" s="25">
+      <c r="M49" s="24">
         <f t="shared" si="1"/>
         <v>803.6</v>
       </c>
@@ -13009,47 +13047,47 @@
       <c r="B50" s="18">
         <v>25</v>
       </c>
-      <c r="C50" s="24">
+      <c r="C50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!C$4)</f>
         <v>773</v>
       </c>
-      <c r="D50" s="24">
+      <c r="D50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!D$4)</f>
         <v>1078</v>
       </c>
-      <c r="E50" s="24">
+      <c r="E50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!E$4)</f>
         <v>746</v>
       </c>
-      <c r="F50" s="24">
+      <c r="F50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!F$4)</f>
         <v>701</v>
       </c>
-      <c r="G50" s="24">
+      <c r="G50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!G$4)</f>
         <v>902</v>
       </c>
-      <c r="H50" s="24">
+      <c r="H50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!H$4)</f>
         <v>709</v>
       </c>
-      <c r="I50" s="24">
+      <c r="I50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!I$4)</f>
         <v>1137</v>
       </c>
-      <c r="J50" s="24">
+      <c r="J50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!J$4)</f>
         <v>484</v>
       </c>
-      <c r="K50" s="24">
+      <c r="K50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!K$4)</f>
         <v>677</v>
       </c>
-      <c r="L50" s="24">
+      <c r="L50" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B50,exec!$L:$L,tabela!L$4)</f>
         <v>882</v>
       </c>
-      <c r="M50" s="25">
+      <c r="M50" s="24">
         <f t="shared" si="1"/>
         <v>808.9</v>
       </c>
@@ -13058,47 +13096,47 @@
       <c r="B51" s="18">
         <v>26</v>
       </c>
-      <c r="C51" s="24">
+      <c r="C51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!C$4)</f>
         <v>893</v>
       </c>
-      <c r="D51" s="24">
+      <c r="D51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!D$4)</f>
         <v>768</v>
       </c>
-      <c r="E51" s="24">
+      <c r="E51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!E$4)</f>
         <v>984</v>
       </c>
-      <c r="F51" s="24">
+      <c r="F51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!F$4)</f>
         <v>943</v>
       </c>
-      <c r="G51" s="24">
+      <c r="G51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!G$4)</f>
         <v>867</v>
       </c>
-      <c r="H51" s="24">
+      <c r="H51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!H$4)</f>
         <v>720</v>
       </c>
-      <c r="I51" s="24">
+      <c r="I51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!I$4)</f>
         <v>923</v>
       </c>
-      <c r="J51" s="24">
+      <c r="J51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!J$4)</f>
         <v>815</v>
       </c>
-      <c r="K51" s="24">
+      <c r="K51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!K$4)</f>
         <v>776</v>
       </c>
-      <c r="L51" s="24">
+      <c r="L51" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B51,exec!$L:$L,tabela!L$4)</f>
         <v>897</v>
       </c>
-      <c r="M51" s="25">
+      <c r="M51" s="24">
         <f t="shared" si="1"/>
         <v>858.6</v>
       </c>
@@ -13107,47 +13145,47 @@
       <c r="B52" s="18">
         <v>27</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!C$4)</f>
         <v>950</v>
       </c>
-      <c r="D52" s="24">
+      <c r="D52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!D$4)</f>
         <v>1133</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!E$4)</f>
         <v>693</v>
       </c>
-      <c r="F52" s="24">
+      <c r="F52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!F$4)</f>
         <v>650</v>
       </c>
-      <c r="G52" s="24">
+      <c r="G52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!G$4)</f>
         <v>885</v>
       </c>
-      <c r="H52" s="24">
+      <c r="H52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!H$4)</f>
         <v>1036</v>
       </c>
-      <c r="I52" s="24">
+      <c r="I52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!I$4)</f>
         <v>718</v>
       </c>
-      <c r="J52" s="24">
+      <c r="J52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!J$4)</f>
         <v>853</v>
       </c>
-      <c r="K52" s="24">
+      <c r="K52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!K$4)</f>
         <v>840</v>
       </c>
-      <c r="L52" s="24">
+      <c r="L52" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B52,exec!$L:$L,tabela!L$4)</f>
         <v>806</v>
       </c>
-      <c r="M52" s="25">
+      <c r="M52" s="24">
         <f t="shared" si="1"/>
         <v>856.4</v>
       </c>
@@ -13156,47 +13194,47 @@
       <c r="B53" s="18">
         <v>28</v>
       </c>
-      <c r="C53" s="24">
+      <c r="C53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!C$4)</f>
         <v>953</v>
       </c>
-      <c r="D53" s="24">
+      <c r="D53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!D$4)</f>
         <v>984</v>
       </c>
-      <c r="E53" s="24">
+      <c r="E53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!E$4)</f>
         <v>1041</v>
       </c>
-      <c r="F53" s="24">
+      <c r="F53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!F$4)</f>
         <v>904</v>
       </c>
-      <c r="G53" s="24">
+      <c r="G53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!G$4)</f>
         <v>984</v>
       </c>
-      <c r="H53" s="24">
+      <c r="H53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!H$4)</f>
         <v>990</v>
       </c>
-      <c r="I53" s="24">
+      <c r="I53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!I$4)</f>
         <v>984</v>
       </c>
-      <c r="J53" s="24">
+      <c r="J53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!J$4)</f>
         <v>699</v>
       </c>
-      <c r="K53" s="24">
+      <c r="K53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!K$4)</f>
         <v>765</v>
       </c>
-      <c r="L53" s="24">
+      <c r="L53" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B53,exec!$L:$L,tabela!L$4)</f>
         <v>990</v>
       </c>
-      <c r="M53" s="25">
+      <c r="M53" s="24">
         <f t="shared" si="1"/>
         <v>929.4</v>
       </c>
@@ -13205,47 +13243,47 @@
       <c r="B54" s="18">
         <v>29</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!C$4)</f>
         <v>803</v>
       </c>
-      <c r="D54" s="24">
+      <c r="D54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!D$4)</f>
         <v>1003</v>
       </c>
-      <c r="E54" s="24">
+      <c r="E54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!E$4)</f>
         <v>916</v>
       </c>
-      <c r="F54" s="24">
+      <c r="F54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!F$4)</f>
         <v>800</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!G$4)</f>
         <v>1112</v>
       </c>
-      <c r="H54" s="24">
+      <c r="H54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!H$4)</f>
         <v>852</v>
       </c>
-      <c r="I54" s="24">
+      <c r="I54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!I$4)</f>
         <v>972</v>
       </c>
-      <c r="J54" s="24">
+      <c r="J54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!J$4)</f>
         <v>1067</v>
       </c>
-      <c r="K54" s="24">
+      <c r="K54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!K$4)</f>
         <v>1049</v>
       </c>
-      <c r="L54" s="24">
+      <c r="L54" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B54,exec!$L:$L,tabela!L$4)</f>
         <v>821</v>
       </c>
-      <c r="M54" s="25">
+      <c r="M54" s="24">
         <f t="shared" si="1"/>
         <v>939.5</v>
       </c>
@@ -13254,47 +13292,47 @@
       <c r="B55" s="18">
         <v>30</v>
       </c>
-      <c r="C55" s="24">
+      <c r="C55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!C$4)</f>
         <v>775</v>
       </c>
-      <c r="D55" s="24">
+      <c r="D55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!D$4)</f>
         <v>929</v>
       </c>
-      <c r="E55" s="24">
+      <c r="E55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!E$4)</f>
         <v>1103</v>
       </c>
-      <c r="F55" s="24">
+      <c r="F55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!F$4)</f>
         <v>853</v>
       </c>
-      <c r="G55" s="24">
+      <c r="G55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!G$4)</f>
         <v>1007</v>
       </c>
-      <c r="H55" s="24">
+      <c r="H55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!H$4)</f>
         <v>754</v>
       </c>
-      <c r="I55" s="24">
+      <c r="I55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!I$4)</f>
         <v>925</v>
       </c>
-      <c r="J55" s="24">
+      <c r="J55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!J$4)</f>
         <v>745</v>
       </c>
-      <c r="K55" s="24">
+      <c r="K55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!K$4)</f>
         <v>828</v>
       </c>
-      <c r="L55" s="24">
+      <c r="L55" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B55,exec!$L:$L,tabela!L$4)</f>
         <v>1003</v>
       </c>
-      <c r="M55" s="25">
+      <c r="M55" s="24">
         <f t="shared" si="1"/>
         <v>892.2</v>
       </c>
@@ -13303,47 +13341,47 @@
       <c r="B56" s="18">
         <v>31</v>
       </c>
-      <c r="C56" s="24">
+      <c r="C56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!C$4)</f>
         <v>1053</v>
       </c>
-      <c r="D56" s="24">
+      <c r="D56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!D$4)</f>
         <v>1079</v>
       </c>
-      <c r="E56" s="24">
+      <c r="E56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!E$4)</f>
         <v>895</v>
       </c>
-      <c r="F56" s="24">
+      <c r="F56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!F$4)</f>
         <v>975</v>
       </c>
-      <c r="G56" s="24">
+      <c r="G56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!G$4)</f>
         <v>751</v>
       </c>
-      <c r="H56" s="24">
+      <c r="H56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!H$4)</f>
         <v>943</v>
       </c>
-      <c r="I56" s="24">
+      <c r="I56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!I$4)</f>
         <v>1091</v>
       </c>
-      <c r="J56" s="24">
+      <c r="J56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!J$4)</f>
         <v>876</v>
       </c>
-      <c r="K56" s="24">
+      <c r="K56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!K$4)</f>
         <v>697</v>
       </c>
-      <c r="L56" s="24">
+      <c r="L56" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B56,exec!$L:$L,tabela!L$4)</f>
         <v>1004</v>
       </c>
-      <c r="M56" s="25">
+      <c r="M56" s="24">
         <f t="shared" si="1"/>
         <v>936.4</v>
       </c>
@@ -13352,47 +13390,47 @@
       <c r="B57" s="18">
         <v>32</v>
       </c>
-      <c r="C57" s="24">
+      <c r="C57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D57" s="24">
+      <c r="D57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E57" s="24">
+      <c r="E57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F57" s="24">
+      <c r="F57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I57" s="24">
+      <c r="I57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="24">
+      <c r="J57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K57" s="24">
+      <c r="K57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L57" s="24">
+      <c r="L57" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B57,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M57" s="25">
+      <c r="M57" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13401,47 +13439,47 @@
       <c r="B58" s="18">
         <v>33</v>
       </c>
-      <c r="C58" s="24">
+      <c r="C58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="24">
+      <c r="D58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="24">
+      <c r="E58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F58" s="24">
+      <c r="F58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G58" s="24">
+      <c r="G58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H58" s="24">
+      <c r="H58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I58" s="24">
+      <c r="I58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J58" s="24">
+      <c r="J58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K58" s="24">
+      <c r="K58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L58" s="24">
+      <c r="L58" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B58,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M58" s="25">
+      <c r="M58" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13450,47 +13488,47 @@
       <c r="B59" s="18">
         <v>34</v>
       </c>
-      <c r="C59" s="24">
+      <c r="C59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D59" s="24">
+      <c r="D59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E59" s="24">
+      <c r="E59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F59" s="24">
+      <c r="F59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G59" s="24">
+      <c r="G59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H59" s="24">
+      <c r="H59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I59" s="24">
+      <c r="I59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J59" s="24">
+      <c r="J59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K59" s="24">
+      <c r="K59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L59" s="24">
+      <c r="L59" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B59,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M59" s="25">
+      <c r="M59" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13499,47 +13537,47 @@
       <c r="B60" s="18">
         <v>35</v>
       </c>
-      <c r="C60" s="24">
+      <c r="C60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D60" s="24">
+      <c r="D60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E60" s="24">
+      <c r="E60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F60" s="24">
+      <c r="F60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G60" s="24">
+      <c r="G60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H60" s="24">
+      <c r="H60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I60" s="24">
+      <c r="I60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J60" s="24">
+      <c r="J60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K60" s="24">
+      <c r="K60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L60" s="24">
+      <c r="L60" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B60,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M60" s="25">
+      <c r="M60" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13548,47 +13586,47 @@
       <c r="B61" s="18">
         <v>36</v>
       </c>
-      <c r="C61" s="24">
+      <c r="C61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D61" s="24">
+      <c r="D61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E61" s="24">
+      <c r="E61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F61" s="24">
+      <c r="F61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G61" s="24">
+      <c r="G61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H61" s="24">
+      <c r="H61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I61" s="24">
+      <c r="I61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J61" s="24">
+      <c r="J61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K61" s="24">
+      <c r="K61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L61" s="24">
+      <c r="L61" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B61,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M61" s="25">
+      <c r="M61" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -13597,47 +13635,47 @@
       <c r="B62" s="18">
         <v>37</v>
       </c>
-      <c r="C62" s="24">
+      <c r="C62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!C$4)</f>
         <v>0</v>
       </c>
-      <c r="D62" s="24">
+      <c r="D62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!D$4)</f>
         <v>0</v>
       </c>
-      <c r="E62" s="24">
+      <c r="E62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!E$4)</f>
         <v>0</v>
       </c>
-      <c r="F62" s="24">
+      <c r="F62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!F$4)</f>
         <v>0</v>
       </c>
-      <c r="G62" s="24">
+      <c r="G62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!G$4)</f>
         <v>0</v>
       </c>
-      <c r="H62" s="24">
+      <c r="H62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!H$4)</f>
         <v>0</v>
       </c>
-      <c r="I62" s="24">
+      <c r="I62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!I$4)</f>
         <v>0</v>
       </c>
-      <c r="J62" s="24">
+      <c r="J62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!J$4)</f>
         <v>0</v>
       </c>
-      <c r="K62" s="24">
+      <c r="K62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!K$4)</f>
         <v>0</v>
       </c>
-      <c r="L62" s="24">
+      <c r="L62" s="23">
         <f>SUMIFS(exec!$E:$E,exec!$C:$C,tabela!$B62,exec!$L:$L,tabela!L$4)</f>
         <v>0</v>
       </c>
-      <c r="M62" s="25">
+      <c r="M62" s="24">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>